<commit_message>
Add error message for value only with spl allowed characters without number or letter
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal5-Files/FAL5-invalidCharacters.xlsx
+++ b/cypress/fixtures/Fal5-Files/FAL5-invalidCharacters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal5-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSWTemp\nmsw-ui\cypress\fixtures\Fal5-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89A75C6-EB7F-4674-AEC1-1BA9DB59D5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EFAA3B-7E05-4CEE-ABFE-B974B468109D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="LOCODES " sheetId="2" r:id="rId3"/>
     <sheet name="ISO 3-letter country codes" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028" iterateCount="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5022,15 +5022,6 @@
     <t>0987654567</t>
   </si>
   <si>
-    <t>SN</t>
-  </si>
-  <si>
-    <t>Rogers</t>
-  </si>
-  <si>
-    <t>Steve</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -5038,6 +5029,15 @@
   </si>
   <si>
     <t>24/12/2024</t>
+  </si>
+  <si>
+    <t>-/</t>
+  </si>
+  <si>
+    <t>/'</t>
+  </si>
+  <si>
+    <t>/:</t>
   </si>
 </sst>
 </file>
@@ -5793,7 +5793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5950,6 +5950,21 @@
     <xf numFmtId="49" fontId="16" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="44" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5992,18 +6007,6 @@
     <xf numFmtId="49" fontId="10" fillId="8" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7168,7 +7171,7 @@
   <dimension ref="A1:AA980"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" customHeight="1"/>
@@ -7191,10 +7194,10 @@
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="75"/>
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
       <c r="H1" s="31"/>
@@ -7218,20 +7221,20 @@
       <c r="Z1" s="35"/>
     </row>
     <row r="2" spans="1:26" ht="30" customHeight="1">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="65"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="72"/>
       <c r="M2" s="3"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -7404,42 +7407,42 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="62" t="s">
         <v>1637</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="63" t="s">
         <v>1638</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="64" t="s">
         <v>1639</v>
       </c>
-      <c r="E6" s="79" t="s">
+      <c r="E6" s="68" t="s">
+        <v>1643</v>
+      </c>
+      <c r="F6" s="63" t="s">
+        <v>1644</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H6" s="62" t="s">
         <v>1640</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="I6" s="63" t="s">
         <v>1641</v>
       </c>
-      <c r="G6" s="79" t="s">
+      <c r="J6" s="63" t="s">
+        <v>1585</v>
+      </c>
+      <c r="K6" s="63" t="s">
+        <v>1585</v>
+      </c>
+      <c r="L6" s="65" t="s">
         <v>1642</v>
       </c>
-      <c r="H6" s="78" t="s">
-        <v>1643</v>
-      </c>
-      <c r="I6" s="79" t="s">
-        <v>1644</v>
-      </c>
-      <c r="J6" s="79" t="s">
-        <v>1585</v>
-      </c>
-      <c r="K6" s="79" t="s">
-        <v>1585</v>
-      </c>
-      <c r="L6" s="81" t="s">
-        <v>1645</v>
-      </c>
-      <c r="M6" s="82"/>
-      <c r="Z6" s="83"/>
+      <c r="M6" s="66"/>
+      <c r="Z6" s="67"/>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="59"/>
@@ -39182,11 +39185,11 @@
       <c r="B1" s="25" t="s">
         <v>1116</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="76" t="s">
         <v>1117</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
       <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6">
@@ -39196,9 +39199,9 @@
       <c r="B2" s="25" t="s">
         <v>1119</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="81"/>
       <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6">
@@ -39208,11 +39211,11 @@
       <c r="B3" s="25" t="s">
         <v>1121</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="82" t="s">
         <v>1122</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="77"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="84"/>
       <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
@@ -41250,17 +41253,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -41497,6 +41489,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EF1FD61-C2E6-4843-9418-343E38DCD8AB}">
   <ds:schemaRefs>
@@ -41506,17 +41509,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8DCF1D7-99F7-4202-82A6-46959FA5E53C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABE1220D-06A4-4F97-A70F-0D90EAC761EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41533,4 +41525,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8DCF1D7-99F7-4202-82A6-46959FA5E53C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>